<commit_message>
last commit before computer dies
</commit_message>
<xml_diff>
--- a/images/Brackets.xlsx
+++ b/images/Brackets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\00School\04College\17Senior\Thesis\Latex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065A7E90-215D-4890-876E-0773FD25401F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF15015-0618-4B12-8EFF-01859BE540D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
   <si>
     <t>Georgia</t>
   </si>
@@ -186,6 +187,12 @@
   </si>
   <si>
     <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Season</t>
   </si>
 </sst>
 </file>
@@ -374,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -398,24 +405,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -424,14 +428,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1111,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1876FCB-6DB9-423A-8CE5-BFA1290FCF13}">
   <dimension ref="A2:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1671,7 +1672,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C59F7E8-88AA-4FE9-B6FA-71F38FE540A6}">
-  <dimension ref="A4:AA41"/>
+  <dimension ref="A4:AA38"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AA13" sqref="P12:AA13"/>
@@ -1692,12 +1693,12 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="14"/>
-      <c r="P4" s="19">
+      <c r="M4" s="1"/>
+      <c r="P4" s="17">
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>33-P4</f>
+        <f t="shared" ref="Q4:Q35" si="0">33-P4</f>
         <v>32</v>
       </c>
       <c r="R4">
@@ -1738,12 +1739,12 @@
       <c r="L5" s="6">
         <v>2</v>
       </c>
-      <c r="M5" s="14"/>
-      <c r="P5" s="19">
+      <c r="M5" s="1"/>
+      <c r="P5" s="17">
         <v>2</v>
       </c>
       <c r="Q5">
-        <f>33-P5</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="R5">
@@ -1778,14 +1779,14 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="16"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="14"/>
-      <c r="P6" s="19">
+      <c r="M6" s="1"/>
+      <c r="P6" s="17">
         <v>3</v>
       </c>
       <c r="Q6">
-        <f>33-P6</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="R6">
@@ -1822,16 +1823,16 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="17"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="12">
         <v>31</v>
       </c>
-      <c r="M7" s="14"/>
-      <c r="P7" s="19">
+      <c r="M7" s="1"/>
+      <c r="P7" s="17">
         <v>4</v>
       </c>
       <c r="Q7">
-        <f>33-P7</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="R7">
@@ -1865,15 +1866,15 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="17"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="14"/>
-      <c r="P8" s="19">
+      <c r="M8" s="1"/>
+      <c r="P8" s="17">
         <v>5</v>
       </c>
       <c r="Q8">
-        <f>33-P8</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="R8">
@@ -1914,12 +1915,12 @@
       <c r="L9" s="6">
         <v>15</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="P9" s="19">
+      <c r="M9" s="1"/>
+      <c r="P9" s="17">
         <v>6</v>
       </c>
       <c r="Q9">
-        <f>33-P9</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="R9">
@@ -1954,14 +1955,14 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="18"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="11"/>
-      <c r="M10" s="14"/>
-      <c r="P10" s="19">
+      <c r="M10" s="1"/>
+      <c r="P10" s="17">
         <v>7</v>
       </c>
       <c r="Q10">
-        <f>33-P10</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="R10">
@@ -2002,12 +2003,12 @@
       <c r="L11" s="12">
         <v>18</v>
       </c>
-      <c r="M11" s="14"/>
-      <c r="P11" s="19">
+      <c r="M11" s="1"/>
+      <c r="P11" s="17">
         <v>8</v>
       </c>
       <c r="Q11">
-        <f>33-P11</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="R11">
@@ -2044,12 +2045,12 @@
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="14"/>
-      <c r="P12" s="19">
+      <c r="M12" s="1"/>
+      <c r="P12" s="17">
         <v>9</v>
       </c>
       <c r="Q12">
-        <f>33-P12</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="R12">
@@ -2082,20 +2083,20 @@
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="17"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="15"/>
       <c r="J13" s="5"/>
       <c r="K13" s="1"/>
       <c r="L13" s="6">
         <v>7</v>
       </c>
-      <c r="M13" s="14"/>
-      <c r="P13" s="19">
+      <c r="M13" s="1"/>
+      <c r="P13" s="17">
         <v>10</v>
       </c>
       <c r="Q13">
-        <f>33-P13</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="R13">
@@ -2126,18 +2127,18 @@
       <c r="D14" s="1"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="16"/>
+      <c r="K14" s="14"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="14"/>
-      <c r="P14" s="19">
+      <c r="M14" s="1"/>
+      <c r="P14" s="17">
         <v>11</v>
       </c>
       <c r="Q14">
-        <f>33-P14</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="R14">
@@ -2170,20 +2171,20 @@
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="2"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="17"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="12">
         <v>26</v>
       </c>
-      <c r="M15" s="14"/>
-      <c r="P15" s="19">
+      <c r="M15" s="1"/>
+      <c r="P15" s="17">
         <v>12</v>
       </c>
       <c r="Q15">
-        <f>33-P15</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="R15">
@@ -2214,18 +2215,18 @@
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="18"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="14"/>
-      <c r="P16" s="19">
+      <c r="M16" s="1"/>
+      <c r="P16" s="17">
         <v>13</v>
       </c>
       <c r="Q16">
-        <f>33-P16</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="R16">
@@ -2258,20 +2259,20 @@
       <c r="D17" s="4"/>
       <c r="E17" s="1"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="5"/>
       <c r="J17" s="1"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6">
         <v>10</v>
       </c>
-      <c r="M17" s="14"/>
-      <c r="P17" s="19">
+      <c r="M17" s="1"/>
+      <c r="P17" s="17">
         <v>14</v>
       </c>
       <c r="Q17">
-        <f>33-P17</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="R17">
@@ -2302,18 +2303,18 @@
       <c r="D18" s="5"/>
       <c r="E18" s="1"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="I18" s="5"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="18"/>
+      <c r="K18" s="16"/>
       <c r="L18" s="11"/>
-      <c r="M18" s="14"/>
-      <c r="P18" s="19">
+      <c r="M18" s="1"/>
+      <c r="P18" s="17">
         <v>15</v>
       </c>
       <c r="Q18">
-        <f>33-P18</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="R18">
@@ -2346,20 +2347,20 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="5"/>
       <c r="J19" s="1"/>
       <c r="K19" s="2"/>
       <c r="L19" s="12">
         <v>23</v>
       </c>
-      <c r="M19" s="14"/>
-      <c r="P19" s="19">
+      <c r="M19" s="1"/>
+      <c r="P19" s="17">
         <v>16</v>
       </c>
       <c r="Q19">
-        <f>33-P19</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="R19">
@@ -2390,18 +2391,18 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="5"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="6"/>
       <c r="M20" s="1"/>
-      <c r="P20" s="19">
+      <c r="P20" s="17">
         <v>17</v>
       </c>
       <c r="Q20">
-        <f>33-P20</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="R20">
@@ -2442,20 +2443,20 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="5"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="6">
         <v>3</v>
       </c>
-      <c r="M21" s="14"/>
-      <c r="P21" s="19">
+      <c r="M21" s="1"/>
+      <c r="P21" s="17">
         <v>18</v>
       </c>
       <c r="Q21">
-        <f>33-P21</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="R21">
@@ -2494,18 +2495,18 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="5"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="16"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="11"/>
-      <c r="M22" s="14"/>
-      <c r="P22" s="19">
+      <c r="M22" s="1"/>
+      <c r="P22" s="17">
         <v>19</v>
       </c>
       <c r="Q22">
-        <f>33-P22</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="R22">
@@ -2546,20 +2547,20 @@
       <c r="D23" s="5"/>
       <c r="E23" s="1"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="5"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="17"/>
+      <c r="K23" s="15"/>
       <c r="L23" s="12">
         <v>30</v>
       </c>
-      <c r="M23" s="14"/>
-      <c r="P23" s="19">
+      <c r="M23" s="1"/>
+      <c r="P23" s="17">
         <v>20</v>
       </c>
       <c r="Q23">
-        <f>33-P23</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="R23">
@@ -2598,18 +2599,18 @@
       <c r="D24" s="5"/>
       <c r="E24" s="1"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="17"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="5"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="14"/>
-      <c r="P24" s="19">
+      <c r="M24" s="1"/>
+      <c r="P24" s="17">
         <v>21</v>
       </c>
       <c r="Q24">
-        <f>33-P24</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="R24">
@@ -2650,20 +2651,20 @@
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="6">
         <v>14</v>
       </c>
-      <c r="M25" s="14"/>
-      <c r="P25" s="19">
+      <c r="M25" s="1"/>
+      <c r="P25" s="17">
         <v>22</v>
       </c>
       <c r="Q25">
-        <f>33-P25</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="R25">
@@ -2702,18 +2703,18 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="18"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="11"/>
-      <c r="M26" s="14"/>
-      <c r="P26" s="19">
+      <c r="M26" s="1"/>
+      <c r="P26" s="17">
         <v>23</v>
       </c>
       <c r="Q26">
-        <f>33-P26</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="R26">
@@ -2754,20 +2755,20 @@
       <c r="D27" s="1"/>
       <c r="E27" s="5"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="2"/>
       <c r="L27" s="12">
         <v>19</v>
       </c>
-      <c r="M27" s="14"/>
-      <c r="P27" s="19">
+      <c r="M27" s="1"/>
+      <c r="P27" s="17">
         <v>24</v>
       </c>
       <c r="Q27">
-        <f>33-P27</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="R27">
@@ -2806,18 +2807,18 @@
       <c r="D28" s="1"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
       <c r="I28" s="10"/>
       <c r="J28" s="5"/>
       <c r="K28" s="1"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="14"/>
-      <c r="P28" s="19">
+      <c r="M28" s="1"/>
+      <c r="P28" s="17">
         <v>25</v>
       </c>
       <c r="Q28">
-        <f>33-P28</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="R28">
@@ -2857,21 +2858,21 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="2"/>
       <c r="J29" s="5"/>
       <c r="K29" s="1"/>
       <c r="L29" s="6">
         <v>6</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="P29" s="19">
+      <c r="M29" s="1"/>
+      <c r="P29" s="17">
         <v>26</v>
       </c>
       <c r="Q29">
-        <f>33-P29</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="R29">
@@ -2909,19 +2910,19 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="16"/>
+      <c r="K30" s="14"/>
       <c r="L30" s="11"/>
-      <c r="M30" s="14"/>
-      <c r="P30" s="19">
+      <c r="M30" s="1"/>
+      <c r="P30" s="17">
         <v>27</v>
       </c>
       <c r="Q30">
-        <f>33-P30</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R30">
@@ -2961,21 +2962,21 @@
       <c r="C31" s="4"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="17"/>
+      <c r="K31" s="15"/>
       <c r="L31" s="12">
         <v>27</v>
       </c>
-      <c r="M31" s="14"/>
-      <c r="P31" s="19">
+      <c r="M31" s="1"/>
+      <c r="P31" s="17">
         <v>28</v>
       </c>
       <c r="Q31">
-        <f>33-P31</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R31">
@@ -3013,19 +3014,19 @@
       <c r="C32" s="1"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="18"/>
+      <c r="J32" s="16"/>
       <c r="K32" s="5"/>
       <c r="L32" s="6"/>
-      <c r="M32" s="14"/>
-      <c r="P32" s="19">
+      <c r="M32" s="1"/>
+      <c r="P32" s="17">
         <v>29</v>
       </c>
       <c r="Q32">
-        <f>33-P32</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R32">
@@ -3065,21 +3066,21 @@
       <c r="C33" s="1"/>
       <c r="D33" s="4"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="5"/>
       <c r="L33" s="6">
         <v>11</v>
       </c>
-      <c r="M33" s="14"/>
-      <c r="P33" s="19">
+      <c r="M33" s="1"/>
+      <c r="P33" s="17">
         <v>30</v>
       </c>
       <c r="Q33">
-        <f>33-P33</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R33">
@@ -3117,19 +3118,19 @@
       <c r="C34" s="1"/>
       <c r="D34" s="5"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="18"/>
+      <c r="K34" s="16"/>
       <c r="L34" s="11"/>
-      <c r="M34" s="14"/>
-      <c r="P34" s="19">
+      <c r="M34" s="1"/>
+      <c r="P34" s="17">
         <v>31</v>
       </c>
       <c r="Q34">
-        <f>33-P34</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R34">
@@ -3169,21 +3170,21 @@
       <c r="C35" s="4"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="2"/>
       <c r="L35" s="12">
         <v>22</v>
       </c>
-      <c r="M35" s="14"/>
-      <c r="P35" s="19">
+      <c r="M35" s="1"/>
+      <c r="P35" s="17">
         <v>32</v>
       </c>
       <c r="Q35">
-        <f>33-P35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R35">
@@ -3221,67 +3222,21 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="14"/>
-      <c r="P36" s="19"/>
+      <c r="M36" s="1"/>
+      <c r="P36" s="17"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="P37" s="19"/>
+      <c r="P37" s="17"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="P38" s="19"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="P38" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3291,7 +3246,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4FDA5A-1FA6-4FB5-874D-8ADC03C2B365}">
-  <dimension ref="B3:G18"/>
+  <dimension ref="B4:G18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D16" sqref="D16:D17"/>
@@ -3306,21 +3261,17 @@
     <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-    </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="20"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="20"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="6" t="s">
         <v>27</v>
@@ -3333,7 +3284,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
       <c r="G6" s="1"/>
@@ -3343,7 +3294,7 @@
       <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5" t="s">
         <v>28</v>
@@ -3355,15 +3306,15 @@
         <v>33</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="22"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="1"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="22"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="19"/>
       <c r="E9" s="8" t="s">
         <v>31</v>
       </c>
@@ -3375,7 +3326,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="14"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="6"/>
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>
@@ -3385,7 +3336,7 @@
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
@@ -3397,15 +3348,15 @@
         <v>35</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="22"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
@@ -3417,7 +3368,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -3427,7 +3378,7 @@
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="5" t="s">
         <v>29</v>
@@ -3439,15 +3390,15 @@
         <v>37</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="22"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="1"/>
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="22"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
@@ -3455,9 +3406,9 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="9"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3474,9 +3425,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426E89DE-FB26-4184-BD37-CBFF7802F4CC}">
-  <dimension ref="B3:I22"/>
+  <dimension ref="B4:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -3490,27 +3441,21 @@
     <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="20"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="20"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="6" t="s">
         <v>46</v>
@@ -3525,7 +3470,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="14"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="2"/>
       <c r="H6" s="5"/>
       <c r="I6" s="1"/>
@@ -3537,7 +3482,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="5" t="s">
         <v>47</v>
@@ -3549,19 +3494,19 @@
         <v>39</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="23"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="23"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
         <v>44</v>
       </c>
@@ -3569,89 +3514,89 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="2:9" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="14"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="2:9" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="25"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="14"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="2:9" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="26"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="14"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="2:9" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="27" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="23"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="27"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="2:9" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="29"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="23"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="28"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="22"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="22"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="19"/>
       <c r="G17" s="1" t="s">
         <v>45</v>
       </c>
@@ -3665,7 +3610,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="14"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="2"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -3677,7 +3622,7 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="14"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="5" t="s">
         <v>13</v>
@@ -3689,19 +3634,19 @@
         <v>42</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
@@ -3709,17 +3654,18 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="I13:I15"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="E10:E11"/>
@@ -3730,8 +3676,110 @@
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD66357-81F2-4B96-BF78-61FF9444A459}">
+  <dimension ref="C3:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started ordered and refactored proper/signatures
</commit_message>
<xml_diff>
--- a/images/Brackets.xlsx
+++ b/images/Brackets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\00School\04College\17Senior\Thesis\Latex\images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leofr\Documents\LeoWork\School\04College\17Senior\Thesis\thesis-tex\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF15015-0618-4B12-8EFF-01859BE540D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48090E46-2DD3-4244-84BF-BC66647BE590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{503DA620-194E-433E-B5EB-5393E7537419}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet5 (2)" sheetId="11" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId10"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>Georgia</t>
   </si>
@@ -114,18 +117,6 @@
     <t>7 Boston</t>
   </si>
   <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
     <t>1 Kanas City</t>
   </si>
   <si>
@@ -194,12 +185,36 @@
   <si>
     <t>Season</t>
   </si>
+  <si>
+    <t>Each number must appear eight times over rows 1,2,8, and 9 and columns 1,2,8, and 9, double counting a number when it appears in both.</t>
+  </si>
+  <si>
+    <t>This double counts numbers exactly when they are in the yellow region, and single counts them exactly when they are in the green region.</t>
+  </si>
+  <si>
+    <t>Thus for all x, 2 * Y(x) + G(x) = 8</t>
+  </si>
+  <si>
+    <t>Let Y(x), G(x), B(x), and O(x) be the number of times x appears in the yellow, green, and blue, and orange regions</t>
+  </si>
+  <si>
+    <t>However, O(x) = 1</t>
+  </si>
+  <si>
+    <t>So Y(x) = B(x)</t>
+  </si>
+  <si>
+    <t>So 2 * B(x) + G(x) = 8</t>
+  </si>
+  <si>
+    <t>Using the same logic on rows and columns 3-7 finds for all x, 2 * B(x) + 2 * O(x) + G(x) = 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +230,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,8 +251,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -377,11 +423,146 @@
         <color auto="1"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -433,6 +614,69 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -759,19 +1003,19 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -780,7 +1024,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
@@ -789,7 +1033,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -798,7 +1042,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -807,7 +1051,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -816,7 +1060,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
@@ -825,7 +1069,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>2</v>
@@ -834,21 +1078,21 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -857,14 +1101,14 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
@@ -873,14 +1117,14 @@
       <c r="D13" s="5"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="5"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -889,14 +1133,14 @@
       <c r="D15" s="4"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="5"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
@@ -905,7 +1149,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -914,6 +1158,682 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075732FB-7749-402F-AAF5-F378F2F73D43}">
+  <dimension ref="B3:AE20"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="R3" s="68"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="68"/>
+      <c r="W3" s="68"/>
+      <c r="X3" s="68"/>
+      <c r="Y3" s="68"/>
+    </row>
+    <row r="4" spans="2:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68">
+        <v>1</v>
+      </c>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+    </row>
+    <row r="5" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="68"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="68">
+        <v>5</v>
+      </c>
+      <c r="U5" s="68"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="68"/>
+      <c r="Y5" s="68"/>
+    </row>
+    <row r="6" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="26"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="6">
+        <v>8</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="68"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="68"/>
+      <c r="Y6" s="68"/>
+    </row>
+    <row r="7" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="26"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="68"/>
+    </row>
+    <row r="8" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6">
+        <v>4</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="26"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="12">
+        <v>11</v>
+      </c>
+      <c r="T8" s="27"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="68"/>
+    </row>
+    <row r="9" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="26"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68">
+        <v>4</v>
+      </c>
+      <c r="U9" s="68"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="68"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="68"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="8">
+        <v>5</v>
+      </c>
+      <c r="L10" s="27"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="26"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="6">
+        <v>9</v>
+      </c>
+      <c r="T10" s="7"/>
+      <c r="U10" s="68"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="68"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="68"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="7"/>
+    </row>
+    <row r="11" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6">
+        <v>2</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="26"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="68"/>
+      <c r="W11" s="68"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="68"/>
+      <c r="AC11" s="67">
+        <v>6</v>
+      </c>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="66"/>
+    </row>
+    <row r="12" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="26"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="12">
+        <v>10</v>
+      </c>
+      <c r="T12" s="27"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="68"/>
+      <c r="W12" s="68"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="68"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="66"/>
+      <c r="AE12" s="27"/>
+    </row>
+    <row r="13" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="6">
+        <v>6</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="26"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="68"/>
+      <c r="T13" s="68"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="68">
+        <v>2</v>
+      </c>
+      <c r="W13" s="68"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="68"/>
+      <c r="AC13" s="66">
+        <v>7</v>
+      </c>
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="67"/>
+    </row>
+    <row r="14" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="26"/>
+      <c r="R14" s="68"/>
+      <c r="S14" s="68"/>
+      <c r="T14" s="68"/>
+      <c r="U14" s="68">
+        <v>3</v>
+      </c>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="68"/>
+    </row>
+    <row r="15" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="8">
+        <v>7</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="26"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="68"/>
+      <c r="T15" s="68">
+        <v>6</v>
+      </c>
+      <c r="U15" s="7"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="68"/>
+      <c r="Y15" s="68"/>
+    </row>
+    <row r="16" spans="2:31" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="26"/>
+      <c r="R16" s="68"/>
+      <c r="S16" s="68"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="68"/>
+      <c r="X16" s="68"/>
+      <c r="Y16" s="68"/>
+    </row>
+    <row r="17" spans="2:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="26"/>
+      <c r="R17" s="68"/>
+      <c r="S17" s="68"/>
+      <c r="T17" s="12">
+        <v>7</v>
+      </c>
+      <c r="U17" s="27"/>
+      <c r="V17" s="68"/>
+      <c r="W17" s="68"/>
+      <c r="X17" s="68"/>
+      <c r="Y17" s="68"/>
+    </row>
+    <row r="18" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="R18" s="68"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="68"/>
+      <c r="U18" s="68"/>
+      <c r="V18" s="68"/>
+      <c r="W18" s="68"/>
+      <c r="X18" s="68"/>
+      <c r="Y18" s="68"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="29"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C071CB8-4A62-48A5-9C91-383608FE5F7C}">
+  <dimension ref="A5:R18"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="13" width="2.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="34"/>
+      <c r="N6" s="56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="35"/>
+      <c r="N7" s="56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="55"/>
+      <c r="N8" s="56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="47"/>
+      <c r="N9" s="56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="50"/>
+      <c r="N10" s="56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="55"/>
+      <c r="N11" s="56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="48"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="47"/>
+      <c r="N12" s="56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="35"/>
+      <c r="N13" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13">
+        <f>SUMPRODUCT(Q14:Q21,R14:R21)</f>
+        <v>32</v>
+      </c>
+      <c r="R13">
+        <f>SUM(R14:R23)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <f>2^P14</f>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <f>2^P15</f>
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <f>2^P16</f>
+        <v>4</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="16:18" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <f>2^P17</f>
+        <v>8</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="16:18" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <f>2^P18</f>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -922,18 +1842,18 @@
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -943,7 +1863,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -955,7 +1875,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="1"/>
@@ -965,7 +1885,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -977,7 +1897,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
@@ -989,7 +1909,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1001,7 +1921,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1013,7 +1933,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1023,7 +1943,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1035,7 +1955,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1047,7 +1967,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -1059,7 +1979,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -1071,7 +1991,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -1081,7 +2001,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
         <v>7</v>
@@ -1093,7 +2013,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1112,19 +2032,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1876FCB-6DB9-423A-8CE5-BFA1290FCF13}">
   <dimension ref="A2:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1142,7 +2060,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="6">
         <v>1</v>
@@ -1166,7 +2084,7 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="7"/>
       <c r="C4" s="1"/>
@@ -1174,9 +2092,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1186,7 +2102,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="8">
         <v>8</v>
@@ -1210,7 +2126,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1"/>
@@ -1219,9 +2135,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="6"/>
@@ -1230,7 +2144,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="6">
         <v>4</v>
@@ -1254,7 +2168,7 @@
       <c r="O7" s="5"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="7"/>
       <c r="C8" s="1"/>
@@ -1262,9 +2176,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="1"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="1"/>
@@ -1274,7 +2186,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
         <v>5</v>
@@ -1298,7 +2210,7 @@
       <c r="O9" s="5"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1"/>
@@ -1308,9 +2220,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="J10" s="5"/>
       <c r="K10" s="1"/>
       <c r="L10" s="6"/>
       <c r="M10" s="1"/>
@@ -1318,7 +2228,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="6">
         <v>3</v>
@@ -1342,7 +2252,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
@@ -1350,9 +2260,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
@@ -1362,7 +2270,7 @@
       <c r="O12" s="5"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
         <v>6</v>
@@ -1386,7 +2294,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1"/>
@@ -1395,9 +2303,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="1"/>
       <c r="L14" s="6"/>
@@ -1406,7 +2312,7 @@
       <c r="O14" s="5"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="6">
         <v>2</v>
@@ -1430,9 +2336,11 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="5"/>
       <c r="E16" s="1"/>
@@ -1440,9 +2348,7 @@
       <c r="G16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="5"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1452,7 +2358,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
         <v>7</v>
@@ -1476,7 +2382,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1504,12 +2410,12 @@
   <dimension ref="A5:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="A5" sqref="A5:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1522,7 +2428,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1535,7 +2441,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -1548,7 +2454,7 @@
       <c r="J7" s="5"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>
@@ -1561,7 +2467,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1574,7 +2480,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1587,7 +2493,7 @@
       <c r="J10" s="5"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -1600,7 +2506,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -1613,7 +2519,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1626,7 +2532,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1639,7 +2545,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1652,7 +2558,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1674,13 +2580,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C59F7E8-88AA-4FE9-B6FA-71F38FE540A6}">
   <dimension ref="A4:AA38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA13" sqref="P12:AA13"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
@@ -1722,7 +2628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="6">
         <v>1</v>
@@ -1768,7 +2674,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="7"/>
       <c r="C6" s="1"/>
@@ -1810,7 +2716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="8">
         <v>32</v>
@@ -1856,7 +2762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="6"/>
       <c r="C8" s="1"/>
@@ -1898,7 +2804,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="6">
         <v>16</v>
@@ -1944,7 +2850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
       <c r="C10" s="1"/>
@@ -1986,7 +2892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
         <v>17</v>
@@ -2032,7 +2938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
@@ -2074,7 +2980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="6">
         <v>8</v>
@@ -2120,7 +3026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="7"/>
       <c r="C14" s="1"/>
@@ -2162,7 +3068,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
         <v>25</v>
@@ -2208,7 +3114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="6"/>
       <c r="C16" s="1"/>
@@ -2250,7 +3156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="6">
         <v>9</v>
@@ -2296,7 +3202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="7"/>
       <c r="C18" s="1"/>
@@ -2338,7 +3244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="8">
         <v>24</v>
@@ -2384,7 +3290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1"/>
@@ -2434,7 +3340,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="6">
         <v>4</v>
@@ -2488,7 +3394,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="7"/>
       <c r="C22" s="1"/>
@@ -2538,7 +3444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="8">
         <v>29</v>
@@ -2592,7 +3498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="6"/>
       <c r="C24" s="1"/>
@@ -2642,7 +3548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="6">
         <v>13</v>
@@ -2696,7 +3602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="7"/>
       <c r="C26" s="1"/>
@@ -2746,7 +3652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="8">
         <v>20</v>
@@ -2800,7 +3706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="6"/>
       <c r="C28" s="1"/>
@@ -2850,7 +3756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="6">
         <v>5</v>
@@ -2904,7 +3810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="7"/>
       <c r="C30" s="1"/>
@@ -2954,7 +3860,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="8">
         <v>28</v>
@@ -3008,7 +3914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="6"/>
       <c r="C32" s="1"/>
@@ -3058,7 +3964,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="6">
         <v>12</v>
@@ -3112,7 +4018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="7"/>
       <c r="C34" s="1"/>
@@ -3162,7 +4068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="8">
         <v>21</v>
@@ -3216,7 +4122,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="6"/>
       <c r="C36" s="1"/>
@@ -3232,10 +4138,10 @@
       <c r="M36" s="1"/>
       <c r="P36" s="17"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="P37" s="17"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="P38" s="17"/>
     </row>
   </sheetData>
@@ -3245,6 +4151,1411 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89773F7F-4D17-4965-AFCD-3A60B3CB582B}">
+  <dimension ref="A4:Y38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="1"/>
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O35" si="0">33-N4</f>
+        <v>32</v>
+      </c>
+      <c r="P4">
+        <v>16</v>
+      </c>
+      <c r="Q4">
+        <v>8</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <f>SUM(O4:$S4)</f>
+        <v>62</v>
+      </c>
+      <c r="Y4">
+        <f>SUM(P4:$S4)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="69">
+        <v>2</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="N5" s="17">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="P5">
+        <v>15</v>
+      </c>
+      <c r="Q5">
+        <v>7</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <f>SUM(O5:$S5)</f>
+        <v>57</v>
+      </c>
+      <c r="Y5">
+        <f>SUM(P5:$S5)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="1"/>
+      <c r="N6" s="17">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>14</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <f>SUM(O6:$S6)</f>
+        <v>53</v>
+      </c>
+      <c r="Y6">
+        <f>SUM(P6:$S6)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="71">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="N7" s="17">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="P7">
+        <v>13</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="X7">
+        <f>SUM(O7:$S7)</f>
+        <v>50</v>
+      </c>
+      <c r="Y7">
+        <f>SUM(P7:$S7)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="1"/>
+      <c r="N8" s="17">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="P8">
+        <v>12</v>
+      </c>
+      <c r="Q8">
+        <v>4</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <f>SUM(O8:$S8)</f>
+        <v>47</v>
+      </c>
+      <c r="Y8">
+        <f>SUM(P8:$S8)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="69">
+        <v>7</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="N9" s="17">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="P9">
+        <v>11</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f>SUM(O9:$S9)</f>
+        <v>44</v>
+      </c>
+      <c r="Y9">
+        <f>SUM(P9:$S9)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="1"/>
+      <c r="N10" s="17">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <f>SUM(O10:$S10)</f>
+        <v>42</v>
+      </c>
+      <c r="Y10">
+        <f>SUM(P10:$S10)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="71">
+        <v>10</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="N11" s="17">
+        <v>8</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="X11">
+        <f>SUM(O11:$S11)</f>
+        <v>41</v>
+      </c>
+      <c r="Y11">
+        <f>SUM(P11:$S11)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="1"/>
+      <c r="N12" s="17">
+        <v>9</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="P12">
+        <v>8</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="X12">
+        <f>SUM(O12:$S12)</f>
+        <v>39</v>
+      </c>
+      <c r="Y12">
+        <f>SUM(P12:$S12)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="N13" s="17">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P13">
+        <v>7</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <f>SUM(O13:$S13)</f>
+        <v>36</v>
+      </c>
+      <c r="Y13">
+        <f>SUM(P13:$S13)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="69">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="N14" s="17">
+        <v>11</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <f>SUM(O14:$S14)</f>
+        <v>34</v>
+      </c>
+      <c r="Y14">
+        <f>SUM(P14:$S14)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="1"/>
+      <c r="N15" s="17">
+        <v>12</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>2</v>
+      </c>
+      <c r="X15">
+        <f>SUM(O15:$S15)</f>
+        <v>33</v>
+      </c>
+      <c r="Y15">
+        <f>SUM(P15:$S15)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="8">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="71">
+        <v>14</v>
+      </c>
+      <c r="K16" s="1"/>
+      <c r="N16" s="17">
+        <v>13</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="X16">
+        <f>SUM(O16:$S16)</f>
+        <v>32</v>
+      </c>
+      <c r="Y16">
+        <f>SUM(P16:$S16)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="1"/>
+      <c r="N17" s="17">
+        <v>14</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P17">
+        <v>3</v>
+      </c>
+      <c r="Q17">
+        <v>6</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <f>SUM(O17:$S17)</f>
+        <v>31</v>
+      </c>
+      <c r="Y17">
+        <f>SUM(P17:$S17)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="69">
+        <v>6</v>
+      </c>
+      <c r="K18" s="1"/>
+      <c r="N18" s="17">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>3</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <f>SUM(O18:$S18)</f>
+        <v>31</v>
+      </c>
+      <c r="Y18">
+        <f>SUM(P18:$S18)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="1"/>
+      <c r="N19" s="17">
+        <v>16</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>8</v>
+      </c>
+      <c r="R19">
+        <v>4</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="X19">
+        <f>SUM(O19:$S19)</f>
+        <v>32</v>
+      </c>
+      <c r="Y19">
+        <f>SUM(P19:$S19)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="8">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="71">
+        <v>11</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="N20" s="17">
+        <v>17</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+      <c r="S20">
+        <v>2</v>
+      </c>
+      <c r="U20">
+        <f>SUM($O20:P20)</f>
+        <v>17</v>
+      </c>
+      <c r="V20">
+        <f>SUM($O20:Q20)</f>
+        <v>25</v>
+      </c>
+      <c r="W20">
+        <f>SUM($O20:R20)</f>
+        <v>29</v>
+      </c>
+      <c r="X20">
+        <f>SUM($O20:S20)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="1"/>
+      <c r="N21" s="17">
+        <v>18</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+      <c r="Q21">
+        <v>7</v>
+      </c>
+      <c r="R21">
+        <v>3</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <f>SUM($O21:P21)</f>
+        <v>17</v>
+      </c>
+      <c r="V21">
+        <f>SUM($O21:Q21)</f>
+        <v>24</v>
+      </c>
+      <c r="W21">
+        <f>SUM($O21:R21)</f>
+        <v>27</v>
+      </c>
+      <c r="X21">
+        <f>SUM($O21:S21)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="1"/>
+      <c r="N22" s="17">
+        <v>19</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>6</v>
+      </c>
+      <c r="R22">
+        <v>2</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <f>SUM($O22:P22)</f>
+        <v>17</v>
+      </c>
+      <c r="V22">
+        <f>SUM($O22:Q22)</f>
+        <v>23</v>
+      </c>
+      <c r="W22">
+        <f>SUM($O22:R22)</f>
+        <v>25</v>
+      </c>
+      <c r="X22">
+        <f>SUM($O22:S22)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="1"/>
+      <c r="N23" s="17">
+        <v>20</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>2</v>
+      </c>
+      <c r="U23">
+        <f>SUM($O23:P23)</f>
+        <v>17</v>
+      </c>
+      <c r="V23">
+        <f>SUM($O23:Q23)</f>
+        <v>22</v>
+      </c>
+      <c r="W23">
+        <f>SUM($O23:R23)</f>
+        <v>23</v>
+      </c>
+      <c r="X23">
+        <f>SUM($O23:S23)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="1"/>
+      <c r="N24" s="17">
+        <v>21</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <f>SUM($O24:P24)</f>
+        <v>17</v>
+      </c>
+      <c r="V24">
+        <f>SUM($O24:Q24)</f>
+        <v>21</v>
+      </c>
+      <c r="W24">
+        <f>SUM($O24:R24)</f>
+        <v>22</v>
+      </c>
+      <c r="X24">
+        <f>SUM($O24:S24)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="1"/>
+      <c r="N25" s="17">
+        <v>22</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>6</v>
+      </c>
+      <c r="Q25">
+        <v>3</v>
+      </c>
+      <c r="R25">
+        <v>2</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <f>SUM($O25:P25)</f>
+        <v>17</v>
+      </c>
+      <c r="V25">
+        <f>SUM($O25:Q25)</f>
+        <v>20</v>
+      </c>
+      <c r="W25">
+        <f>SUM($O25:R25)</f>
+        <v>22</v>
+      </c>
+      <c r="X25">
+        <f>SUM($O25:S25)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="1"/>
+      <c r="N26" s="17">
+        <v>23</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P26">
+        <v>7</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26">
+        <v>3</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <f>SUM($O26:P26)</f>
+        <v>17</v>
+      </c>
+      <c r="V26">
+        <f>SUM($O26:Q26)</f>
+        <v>19</v>
+      </c>
+      <c r="W26">
+        <f>SUM($O26:R26)</f>
+        <v>22</v>
+      </c>
+      <c r="X26">
+        <f>SUM($O26:S26)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="1"/>
+      <c r="N27" s="17">
+        <v>24</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P27">
+        <v>8</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>4</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="U27">
+        <f>SUM($O27:P27)</f>
+        <v>17</v>
+      </c>
+      <c r="V27">
+        <f>SUM($O27:Q27)</f>
+        <v>18</v>
+      </c>
+      <c r="W27">
+        <f>SUM($O27:R27)</f>
+        <v>22</v>
+      </c>
+      <c r="X27">
+        <f>SUM($O27:S27)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="67"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="1"/>
+      <c r="N28" s="17">
+        <v>25</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P28">
+        <v>9</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>4</v>
+      </c>
+      <c r="S28">
+        <v>2</v>
+      </c>
+      <c r="U28">
+        <f>SUM($O28:P28)</f>
+        <v>17</v>
+      </c>
+      <c r="V28">
+        <f>SUM($O28:Q28)</f>
+        <v>18</v>
+      </c>
+      <c r="W28">
+        <f>SUM($O28:R28)</f>
+        <v>22</v>
+      </c>
+      <c r="X28">
+        <f>SUM($O28:S28)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="N29" s="17">
+        <v>26</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P29">
+        <v>10</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29">
+        <v>3</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="U29">
+        <f>SUM($O29:P29)</f>
+        <v>17</v>
+      </c>
+      <c r="V29">
+        <f>SUM($O29:Q29)</f>
+        <v>19</v>
+      </c>
+      <c r="W29">
+        <f>SUM($O29:R29)</f>
+        <v>22</v>
+      </c>
+      <c r="X29">
+        <f>SUM($O29:S29)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="N30" s="17">
+        <v>27</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P30">
+        <v>11</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>2</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f>SUM($O30:P30)</f>
+        <v>17</v>
+      </c>
+      <c r="V30">
+        <f>SUM($O30:Q30)</f>
+        <v>20</v>
+      </c>
+      <c r="W30">
+        <f>SUM($O30:R30)</f>
+        <v>22</v>
+      </c>
+      <c r="X30">
+        <f>SUM($O30:S30)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="N31" s="17">
+        <v>28</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P31">
+        <v>12</v>
+      </c>
+      <c r="Q31">
+        <v>4</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <f>SUM($O31:P31)</f>
+        <v>17</v>
+      </c>
+      <c r="V31">
+        <f>SUM($O31:Q31)</f>
+        <v>21</v>
+      </c>
+      <c r="W31">
+        <f>SUM($O31:R31)</f>
+        <v>22</v>
+      </c>
+      <c r="X31">
+        <f>SUM($O31:S31)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="N32" s="17">
+        <v>29</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>13</v>
+      </c>
+      <c r="Q32">
+        <v>5</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="U32">
+        <f>SUM($O32:P32)</f>
+        <v>17</v>
+      </c>
+      <c r="V32">
+        <f>SUM($O32:Q32)</f>
+        <v>22</v>
+      </c>
+      <c r="W32">
+        <f>SUM($O32:R32)</f>
+        <v>23</v>
+      </c>
+      <c r="X32">
+        <f>SUM($O32:S32)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="N33" s="17">
+        <v>30</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P33">
+        <v>14</v>
+      </c>
+      <c r="Q33">
+        <v>6</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <f>SUM($O33:P33)</f>
+        <v>17</v>
+      </c>
+      <c r="V33">
+        <f>SUM($O33:Q33)</f>
+        <v>23</v>
+      </c>
+      <c r="W33">
+        <f>SUM($O33:R33)</f>
+        <v>25</v>
+      </c>
+      <c r="X33">
+        <f>SUM($O33:S33)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="N34" s="17">
+        <v>31</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P34">
+        <v>15</v>
+      </c>
+      <c r="Q34">
+        <v>7</v>
+      </c>
+      <c r="R34">
+        <v>3</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <f>SUM($O34:P34)</f>
+        <v>17</v>
+      </c>
+      <c r="V34">
+        <f>SUM($O34:Q34)</f>
+        <v>24</v>
+      </c>
+      <c r="W34">
+        <f>SUM($O34:R34)</f>
+        <v>27</v>
+      </c>
+      <c r="X34">
+        <f>SUM($O34:S34)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="N35" s="17">
+        <v>32</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <v>16</v>
+      </c>
+      <c r="Q35">
+        <v>8</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="U35">
+        <f>SUM($O35:P35)</f>
+        <v>17</v>
+      </c>
+      <c r="V35">
+        <f>SUM($O35:Q35)</f>
+        <v>25</v>
+      </c>
+      <c r="W35">
+        <f>SUM($O35:R35)</f>
+        <v>29</v>
+      </c>
+      <c r="X35">
+        <f>SUM($O35:S35)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="N36" s="17"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N37" s="17"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="N38" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4FDA5A-1FA6-4FB5-874D-8ADC03C2B365}">
   <dimension ref="B4:G18"/>
   <sheetViews>
@@ -3252,16 +5563,16 @@
       <selection activeCell="D16" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3269,19 +5580,19 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -3289,21 +5600,21 @@
       <c r="F6" s="5"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="19"/>
@@ -3311,19 +5622,19 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="19"/>
       <c r="E9" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -3331,21 +5642,21 @@
       <c r="F10" s="1"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="19"/>
@@ -3353,19 +5664,19 @@
       <c r="F12" s="1"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="19"/>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -3373,21 +5684,21 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="19"/>
@@ -3395,17 +5706,17 @@
       <c r="F16" s="4"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="19"/>
       <c r="E17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -3423,7 +5734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426E89DE-FB26-4184-BD37-CBFF7802F4CC}">
   <dimension ref="B4:I22"/>
   <sheetViews>
@@ -3431,17 +5742,17 @@
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="2.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3451,21 +5762,21 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -3475,23 +5786,23 @@
       <c r="H6" s="5"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="19"/>
@@ -3501,21 +5812,21 @@
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="19"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="2:9" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -3525,7 +5836,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="2:9" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -3535,7 +5846,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="2:9" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -3545,10 +5856,10 @@
       <c r="H12" s="1"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="2:9" ht="5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" ht="4.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="25"/>
@@ -3556,10 +5867,10 @@
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
       <c r="I13" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="14"/>
       <c r="C14" s="22"/>
       <c r="D14" s="25"/>
@@ -3569,7 +5880,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="2:9" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:9" ht="4.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="18"/>
       <c r="C15" s="23"/>
       <c r="D15" s="25"/>
@@ -3579,9 +5890,9 @@
       <c r="H15" s="1"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="1"/>
@@ -3591,21 +5902,21 @@
       <c r="H16" s="1"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="19"/>
       <c r="G17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -3615,7 +5926,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
       <c r="C19" s="1" t="s">
         <v>13</v>
@@ -3629,9 +5940,9 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="19"/>
@@ -3641,7 +5952,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="19"/>
@@ -3653,7 +5964,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -3665,23 +5976,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD66357-81F2-4B96-BF78-61FF9444A459}">
   <dimension ref="C3:F16"/>
   <sheetViews>
@@ -3689,91 +6000,91 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>

</xml_diff>